<commit_message>
Traduction de l'interface utilisateur.
Signed-off-by: Martin St-Pierre <martin.st-pierre@sct.gouv.qc.ca>
</commit_message>
<xml_diff>
--- a/docs/datamodel/Vaccine Credential Dataset Proposed.xlsx
+++ b/docs/datamodel/Vaccine Credential Dataset Proposed.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flihp/GitHub/dts-vc-issuer-service/docs/datamodel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Documents/GitHub/bradhead/dts-vc-issuer-service/docs/datamodel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D745A7-1A40-1B45-A79B-55AF23CF8AF3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3729CDBE-CE4D-D44D-B1F6-D87138CA3265}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32780" yWindow="1900" windowWidth="30720" windowHeight="18700" activeTab="1" xr2:uid="{A2CBB3ED-6878-C142-8C75-27C6DECA9DD3}"/>
+    <workbookView xWindow="2920" yWindow="3700" windowWidth="34960" windowHeight="20700" xr2:uid="{A2CBB3ED-6878-C142-8C75-27C6DECA9DD3}"/>
   </bookViews>
   <sheets>
-    <sheet name="VC for Vax EN-CA" sheetId="2" r:id="rId1"/>
-    <sheet name="VC pour Vax FR-CA" sheetId="1" r:id="rId2"/>
+    <sheet name="VC for Vax" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
   <si>
     <t>Data Element</t>
   </si>
@@ -109,6 +108,9 @@
     <t>ISO 3166</t>
   </si>
   <si>
+    <t>Admnistration Centre</t>
+  </si>
+  <si>
     <t>The name of the vaccination facility responsible</t>
   </si>
   <si>
@@ -236,99 +238,6 @@
   </si>
   <si>
     <t>As discrete fields</t>
-  </si>
-  <si>
-    <t>Nom complet</t>
-  </si>
-  <si>
-    <t>Date de naissance</t>
-  </si>
-  <si>
-    <t>Identifiant unique du sujet</t>
-  </si>
-  <si>
-    <t>Vaccin administré</t>
-  </si>
-  <si>
-    <t>Marque du vaccin</t>
-  </si>
-  <si>
-    <t>Fabricant du vaccin</t>
-  </si>
-  <si>
-    <t>Maladie</t>
-  </si>
-  <si>
-    <t>Numéro de lot du vaccin</t>
-  </si>
-  <si>
-    <t>Date de vaccination</t>
-  </si>
-  <si>
-    <t>Numéro de la dose</t>
-  </si>
-  <si>
-    <t>Pour les vaccins multidoses, ce numéro est obligatoire.</t>
-  </si>
-  <si>
-    <t>Pays d'administration</t>
-  </si>
-  <si>
-    <t>Administration Centre</t>
-  </si>
-  <si>
-    <t>Centre de vaccination</t>
-  </si>
-  <si>
-    <t>Date  de la prochaine dose</t>
-  </si>
-  <si>
-    <t>Le nom LÉGAL complet du sujet</t>
-  </si>
-  <si>
-    <t>Date de naissance du sujet</t>
-  </si>
-  <si>
-    <t>L'identifiant unique de la personne vaccinée. Recommander le PHN ou le MRN et l'ID de l'établissement</t>
-  </si>
-  <si>
-    <t>Description générique et codification du vaccin</t>
-  </si>
-  <si>
-    <t>La marque ou le nom commercial utilisé pour désigner le vaccin</t>
-  </si>
-  <si>
-    <t>Nom du fabricant du vaccin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restreint à la COVID-19 </t>
-  </si>
-  <si>
-    <t>Numéro de lot ou de lot de fabrication</t>
-  </si>
-  <si>
-    <t>La date à laquelle la vaccination a eu lieu</t>
-  </si>
-  <si>
-    <t>Le pays dans lequel la vaccination a eu lieu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le nom de l'établissement responsable de la vaccination </t>
-  </si>
-  <si>
-    <t>Date de la prochaine dose recommandée à compléter avant. Ou pas avant la date.</t>
-  </si>
-  <si>
-    <t>* Recommane l'utilisation de la banque de la RAMQ pour le nom légal complet qui sera utilisé pour l'identité numérique</t>
-  </si>
-  <si>
-    <t>* Recommande l'utilisation du numéro d'assurance maladie pour l'identifiant unique du sujet</t>
-  </si>
-  <si>
-    <t>Sujet</t>
-  </si>
-  <si>
-    <t>Vaccin</t>
   </si>
 </sst>
 </file>
@@ -454,25 +363,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Century Gothic"/>
-        <family val="1"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <b/>
@@ -505,24 +396,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94BDA654-4492-374D-8399-3495CD684B1A}" name="Table13" displayName="Table13" ref="B1:H15" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="B1:H15" xr:uid="{EE10E400-4092-574C-8F57-A0E94CE2B997}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{940C00E2-10AF-CB42-9087-051712366750}" name="Data Element"/>
-    <tableColumn id="2" xr3:uid="{03F91679-9B87-504E-AF30-5F34572DF135}" name="Description"/>
-    <tableColumn id="3" xr3:uid="{B8A41433-21E9-0B49-95D9-A1301A80BEA2}" name="WHO Spec"/>
-    <tableColumn id="4" xr3:uid="{EBE50308-9BBA-0041-8CF1-EAB49F9228FF}" name="Linux Foundation CCI SB Attribute Name"/>
-    <tableColumn id="5" xr3:uid="{B3FBA8AD-A161-2C46-AD4B-84B1B5C7057C}" name="Recommendation"/>
-    <tableColumn id="7" xr3:uid="{024E6044-0122-B34C-876C-CA79E1EDE6DB}" name="Data Type"/>
-    <tableColumn id="6" xr3:uid="{17BEE056-7BBD-B847-9A60-D2983DE68320}" name="Code Set"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6565A7B3-0796-C048-A77F-9BBA4E2A9B98}" name="Table1" displayName="Table1" ref="B1:H15" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B1:H15" xr:uid="{EE10E400-4092-574C-8F57-A0E94CE2B997}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6565A7B3-0796-C048-A77F-9BBA4E2A9B98}" name="Table1" displayName="Table1" ref="B1:H14" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B1:H14" xr:uid="{EE10E400-4092-574C-8F57-A0E94CE2B997}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{26BEC74E-E38F-3F4C-A2E4-5E74313CB8BD}" name="Data Element"/>
     <tableColumn id="2" xr3:uid="{197E5409-28C8-5743-8776-663EF3F94EE8}" name="Description"/>
@@ -811,11 +686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A0D69F9-587B-DA47-9876-647CF15A9062}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2121A08C-7811-7A48-9C28-8CC9C01BF362}">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -823,12 +698,10 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="73.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="8" width="28.7109375" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" customWidth="1"/>
+    <col min="6" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="9" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
@@ -843,7 +716,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>14</v>
@@ -858,7 +731,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -870,46 +743,46 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -918,13 +791,13 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
@@ -932,7 +805,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -944,13 +817,13 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
@@ -962,22 +835,22 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -992,40 +865,40 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1034,19 +907,19 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
         <v>6</v>
@@ -1054,7 +927,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>18</v>
@@ -1066,16 +939,16 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1090,22 +963,22 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -1114,13 +987,13 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" t="s">
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H12" t="s">
         <v>23</v>
@@ -1129,441 +1002,59 @@
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F14" t="s">
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2121A08C-7811-7A48-9C28-8CC9C01BF362}">
-  <dimension ref="A1:I17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="85" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" t="s">
-        <v>51</v>
-      </c>
-      <c r="H7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>